<commit_message>
Inventario ciclico, inv cierre semana y compra export
</commit_message>
<xml_diff>
--- a/public/application/files/jasper/templates/cierresemana.xlsx
+++ b/public/application/files/jasper/templates/cierresemana.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14680" tabRatio="500"/>
+    <workbookView xWindow="-34900" yWindow="0" windowWidth="28420" windowHeight="16640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>{compania:nombre}</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>{col:veinte}</t>
+  </si>
+  <si>
+    <t>{col:veintiuno}</t>
   </si>
 </sst>
 </file>
@@ -180,7 +183,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -203,45 +206,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -275,8 +241,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -291,6 +263,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -300,14 +275,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -324,6 +295,9 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -340,6 +314,9 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -669,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:U6"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -682,165 +659,171 @@
     <col min="17" max="17" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="28">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:22" ht="28">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
     </row>
-    <row r="2" spans="1:21" ht="28">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:22" ht="28">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
     </row>
-    <row r="3" spans="1:21" ht="28">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:22" ht="28">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:22">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
       <c r="M4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="N4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
     </row>
-    <row r="5" spans="1:21" ht="18">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:22" ht="18">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:22">
       <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="11"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="10"/>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:22">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -901,6 +884,9 @@
       </c>
       <c r="U7" s="2" t="s">
         <v>29</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -908,11 +894,11 @@
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="H4:L4"/>
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="A2:U2"/>
-    <mergeCell ref="A3:U3"/>
-    <mergeCell ref="N4:U4"/>
-    <mergeCell ref="A5:U5"/>
+    <mergeCell ref="A1:V1"/>
+    <mergeCell ref="A2:V2"/>
+    <mergeCell ref="A3:V3"/>
+    <mergeCell ref="N4:V4"/>
+    <mergeCell ref="A5:V5"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
inventario mes semana e inventario ciclico
</commit_message>
<xml_diff>
--- a/public/application/files/jasper/templates/cierresemana.xlsx
+++ b/public/application/files/jasper/templates/cierresemana.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-34900" yWindow="0" windowWidth="28420" windowHeight="16640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>{compania:nombre}</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>{col:veintiuno}</t>
+  </si>
+  <si>
+    <t>{col:veintidos}</t>
   </si>
 </sst>
 </file>
@@ -183,7 +186,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -206,8 +209,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -247,8 +259,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -260,25 +274,34 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -298,6 +321,7 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -317,6 +341,7 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -646,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -659,178 +684,184 @@
     <col min="17" max="17" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="28">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:23" ht="28">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
     </row>
-    <row r="2" spans="1:22" ht="28">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:23" ht="28">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
     </row>
-    <row r="3" spans="1:22" ht="28">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:23" ht="28">
+      <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:23">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
       <c r="G4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
       <c r="M4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
     </row>
-    <row r="5" spans="1:22" ht="18">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:23" ht="18">
+      <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
     </row>
-    <row r="6" spans="1:22">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="10"/>
+    <row r="6" spans="1:23">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:23">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
@@ -887,6 +918,9 @@
       </c>
       <c r="V7" s="2" t="s">
         <v>30</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -894,11 +928,11 @@
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="H4:L4"/>
-    <mergeCell ref="A1:V1"/>
-    <mergeCell ref="A2:V2"/>
-    <mergeCell ref="A3:V3"/>
-    <mergeCell ref="N4:V4"/>
-    <mergeCell ref="A5:V5"/>
+    <mergeCell ref="A1:W1"/>
+    <mergeCell ref="A2:W2"/>
+    <mergeCell ref="A3:W3"/>
+    <mergeCell ref="N4:W4"/>
+    <mergeCell ref="A5:W5"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>